<commit_message>
Update data and visualizations to most recent date available
</commit_message>
<xml_diff>
--- a/Following Trends in Collsion Incidents in Montgomery County/moco_crashes_march2.xlsx
+++ b/Following Trends in Collsion Incidents in Montgomery County/moco_crashes_march2.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagui\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagui\Documents\GitHub\J_Aguirre_portfolio\Following Trends in Collsion Incidents in Montgomery County\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4114316B-6635-4198-88BD-8FE04B97D547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9EDC9E-0F20-4025-9A90-482AFE4327D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="moco_crashes_march" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,15 +684,6 @@
     <xf numFmtId="9" fontId="19" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,6 +714,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,7 +818,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Reported Crash Incidents in Montgomery County from March 1-19, 2020</a:t>
+              <a:t>Reported Crash Incidents in Montgomery County from March 1-30, 2020</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -850,8 +858,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.6524429510272585E-2"/>
-          <c:y val="0.13410719076959129"/>
+          <c:x val="3.6524421094104587E-2"/>
+          <c:y val="0.1363883085420666"/>
           <c:w val="0.93976512213154817"/>
           <c:h val="0.70897382513145424"/>
         </c:manualLayout>
@@ -946,10 +954,10 @@
           </c:dPt>
           <c:yVal>
             <c:numRef>
-              <c:f>moco_crashes_march!$B$40:$B$58</c:f>
+              <c:f>moco_crashes_march!$B$62:$B$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>21</c:v>
                 </c:pt>
@@ -1007,6 +1015,39 @@
                 <c:pt idx="18">
                   <c:v>5</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1032,6 +1073,7 @@
         <c:axId val="142275695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="31"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1040,8 +1082,9 @@
         <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1754,16 +1797,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>191384</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>42270</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>604517</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>53746</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>490980</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>147292</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>295890</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>158768</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1833,12 +1876,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.20695</cdr:x>
-      <cdr:y>0.55263</cdr:y>
+      <cdr:x>0.11632</cdr:x>
+      <cdr:y>0.57324</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.3328</cdr:x>
-      <cdr:y>0.73474</cdr:y>
+      <cdr:x>0.24217</cdr:x>
+      <cdr:y>0.75535</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1853,8 +1896,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2292975" y="3188375"/>
-          <a:ext cx="1394381" cy="1050695"/>
+          <a:off x="1340384" y="3191555"/>
+          <a:ext cx="1450173" cy="1013907"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1914,12 +1957,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.73129</cdr:x>
-      <cdr:y>0.71738</cdr:y>
+      <cdr:x>0.44746</cdr:x>
+      <cdr:y>0.47622</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.8468</cdr:x>
-      <cdr:y>0.88507</cdr:y>
+      <cdr:x>0.56297</cdr:x>
+      <cdr:y>0.64391</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1934,8 +1977,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8398230" y="3822971"/>
-          <a:ext cx="1326563" cy="893596"/>
+          <a:off x="5156044" y="2651369"/>
+          <a:ext cx="1331025" cy="933623"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2067,12 +2110,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.79688</cdr:x>
-      <cdr:y>0.52064</cdr:y>
+      <cdr:x>0.87655</cdr:x>
+      <cdr:y>0.79066</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.87339</cdr:x>
-      <cdr:y>0.63556</cdr:y>
+      <cdr:x>0.95306</cdr:x>
+      <cdr:y>0.90558</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2087,8 +2130,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="9151400" y="2774521"/>
-          <a:ext cx="878734" cy="612425"/>
+          <a:off x="10100544" y="4402034"/>
+          <a:ext cx="881627" cy="639823"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2172,7 +2215,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>3/17</a:t>
+            <a:t>3/30</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -2191,23 +2234,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Saint</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Patrick's Day.</a:t>
+            <a:t> Stay-At-Home order directed</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2220,12 +2247,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.54166</cdr:x>
-      <cdr:y>0.50409</cdr:y>
+      <cdr:x>0.32555</cdr:x>
+      <cdr:y>0.20109</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.65717</cdr:x>
-      <cdr:y>0.67177</cdr:y>
+      <cdr:x>0.44106</cdr:x>
+      <cdr:y>0.36877</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2240,8 +2267,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6001470" y="2908300"/>
-          <a:ext cx="1279853" cy="967446"/>
+          <a:off x="3751293" y="1119589"/>
+          <a:ext cx="1331026" cy="933567"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2819,16 +2846,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E32" zoomScale="97" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="83" workbookViewId="0">
       <selection activeCell="G5" sqref="G5:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
   </cols>
@@ -2877,13 +2904,13 @@
       <c r="B5">
         <v>27</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="9"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21"/>
     </row>
     <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -2892,19 +2919,19 @@
       <c r="B6">
         <v>36</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2918,20 +2945,20 @@
       <c r="G7" s="3">
         <v>2018</v>
       </c>
-      <c r="H7" s="14">
-        <f>AVERAGE(B2:B20)</f>
-        <v>30.210526315789473</v>
+      <c r="H7" s="11">
+        <f>AVERAGE(B2:B31)</f>
+        <v>29.4</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="4">
-        <f>MIN(B2:B20)</f>
-        <v>17</v>
+        <f>MIN(B2:B31)</f>
+        <v>16</v>
       </c>
       <c r="K7" s="5">
-        <f>MAX(B2:B20)</f>
-        <v>40</v>
+        <f>MAX(B2:B31)</f>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2944,21 +2971,21 @@
       <c r="G8" s="3">
         <v>2019</v>
       </c>
-      <c r="H8" s="14">
-        <f>AVERAGE(B21:B39)</f>
-        <v>28.526315789473685</v>
+      <c r="H8" s="11">
+        <f>AVERAGE(B32:B61)</f>
+        <v>30.633333333333333</v>
       </c>
       <c r="I8" s="6">
         <f>((H8-H7)/H7)</f>
-        <v>-5.5749128919860565E-2</v>
+        <v>4.1950113378684845E-2</v>
       </c>
       <c r="J8" s="4">
-        <f>MIN(B21:B39)</f>
+        <f>MIN(B32:B61)</f>
         <v>19</v>
       </c>
       <c r="K8" s="5">
-        <f>MAX(B21:B39)</f>
-        <v>38</v>
+        <f>MAX(B32:B61)</f>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2968,23 +2995,23 @@
       <c r="B9">
         <v>39</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="14">
         <v>2020</v>
       </c>
-      <c r="H9" s="18">
-        <f>AVERAGE(B40:B58)</f>
-        <v>20.94736842105263</v>
-      </c>
-      <c r="I9" s="19">
+      <c r="H9" s="15">
+        <f>AVERAGE(B62:B91)</f>
+        <v>17.266666666666666</v>
+      </c>
+      <c r="I9" s="16">
         <f>((H9-H8)/H8)</f>
-        <v>-0.26568265682656833</v>
-      </c>
-      <c r="J9" s="20">
-        <f>MIN(B40:B58)</f>
+        <v>-0.4363438520130577</v>
+      </c>
+      <c r="J9" s="17">
+        <f>MIN(B62:B91)</f>
         <v>2</v>
       </c>
-      <c r="K9" s="21">
-        <f>MAX(B40:B58)</f>
+      <c r="K9" s="18">
+        <f>MAX(B62:B91)</f>
         <v>41</v>
       </c>
     </row>
@@ -2995,13 +3022,13 @@
       <c r="B10">
         <v>32</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -3085,55 +3112,55 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43525</v>
+        <v>43179</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43526</v>
+        <v>43180</v>
       </c>
       <c r="B22">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43527</v>
+        <v>43181</v>
       </c>
       <c r="B23">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43528</v>
+        <v>43182</v>
       </c>
       <c r="B24">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43529</v>
+        <v>43183</v>
       </c>
       <c r="B25">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43530</v>
+        <v>43184</v>
       </c>
       <c r="B26">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43531</v>
+        <v>43185</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -3141,250 +3168,514 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43532</v>
+        <v>43186</v>
       </c>
       <c r="B28">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43533</v>
+        <v>43187</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43534</v>
+        <v>43188</v>
       </c>
       <c r="B30">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43535</v>
+        <v>43189</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43536</v>
+        <v>43525</v>
       </c>
       <c r="B32">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43537</v>
+        <v>43526</v>
       </c>
       <c r="B33">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43538</v>
+        <v>43527</v>
       </c>
       <c r="B34">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43539</v>
+        <v>43528</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>43540</v>
+        <v>43529</v>
       </c>
       <c r="B36">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>43541</v>
+        <v>43530</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>43542</v>
+        <v>43531</v>
       </c>
       <c r="B38">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>43543</v>
+        <v>43532</v>
       </c>
       <c r="B39">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>43891</v>
+        <v>43533</v>
       </c>
       <c r="B40">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>43892</v>
+        <v>43534</v>
       </c>
       <c r="B41">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>43893</v>
+        <v>43535</v>
       </c>
       <c r="B42">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>43894</v>
+        <v>43536</v>
       </c>
       <c r="B43">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43895</v>
+        <v>43537</v>
       </c>
       <c r="B44">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43896</v>
+        <v>43538</v>
       </c>
       <c r="B45">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>43897</v>
+        <v>43539</v>
       </c>
       <c r="B46">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>43898</v>
+        <v>43540</v>
       </c>
       <c r="B47">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>43899</v>
+        <v>43541</v>
       </c>
       <c r="B48">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>43900</v>
+        <v>43542</v>
       </c>
       <c r="B49">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>43901</v>
+        <v>43543</v>
       </c>
       <c r="B50">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>43902</v>
+        <v>43544</v>
       </c>
       <c r="B51">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>43903</v>
+        <v>43545</v>
       </c>
       <c r="B52">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>43904</v>
+        <v>43546</v>
       </c>
       <c r="B53">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>43905</v>
+        <v>43547</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>43906</v>
+        <v>43548</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>43907</v>
+        <v>43549</v>
       </c>
       <c r="B56">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>43908</v>
+        <v>43550</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
+        <v>43551</v>
+      </c>
+      <c r="B58">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43552</v>
+      </c>
+      <c r="B59">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43553</v>
+      </c>
+      <c r="B60">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43554</v>
+      </c>
+      <c r="B61">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43892</v>
+      </c>
+      <c r="B63">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43893</v>
+      </c>
+      <c r="B64">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43894</v>
+      </c>
+      <c r="B65">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43895</v>
+      </c>
+      <c r="B66">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43896</v>
+      </c>
+      <c r="B67">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>43897</v>
+      </c>
+      <c r="B68">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B69">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B70">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B71">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43901</v>
+      </c>
+      <c r="B72">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43902</v>
+      </c>
+      <c r="B73">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>43903</v>
+      </c>
+      <c r="B74">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>43904</v>
+      </c>
+      <c r="B75">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>43905</v>
+      </c>
+      <c r="B76">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>43906</v>
+      </c>
+      <c r="B77">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43907</v>
+      </c>
+      <c r="B78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>43909</v>
       </c>
-      <c r="B58">
+      <c r="B80">
         <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>43910</v>
+      </c>
+      <c r="B81">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>43911</v>
+      </c>
+      <c r="B82">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B83">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B85">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B88">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B89">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B91">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>